<commit_message>
update: Product-comparision-> company section UI
</commit_message>
<xml_diff>
--- a/public/data.xlsx
+++ b/public/data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Sheet-1"/>
@@ -17,6 +17,60 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5125" uniqueCount="1660">
   <si>
+    <t>Aditya Birla Nifty 50 Index</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Axis Blue Chip Fund</t>
+  </si>
+  <si>
+    <t>Axis ESG Integration Strategy Fund</t>
+  </si>
+  <si>
+    <t>Axis ESG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A </t>
+  </si>
+  <si>
+    <t>Axis Flexi Cap Fund</t>
+  </si>
+  <si>
+    <t>B+</t>
+  </si>
+  <si>
+    <t>Axis Focused Fund</t>
+  </si>
+  <si>
+    <t>Axis Growth Opportunities Fund</t>
+  </si>
+  <si>
+    <t>Axis Multi Cap Fund</t>
+  </si>
+  <si>
+    <t>DSP Flexi Cap Fund</t>
+  </si>
+  <si>
+    <t>DSP Multi Cap Fund</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>DSP Nifty Next 50 Index Fund</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>DSP Quant Fund</t>
+  </si>
+  <si>
+    <t>DSP Value Fund</t>
+  </si>
+  <si>
     <t>Fund Name</t>
   </si>
   <si>
@@ -29,175 +83,121 @@
     <t>Grade</t>
   </si>
   <si>
+    <t>HDFC Flexi Cap Fund</t>
+  </si>
+  <si>
+    <t>HDFC Large Cap and Mid Cap Fund</t>
+  </si>
+  <si>
+    <t>HDFC Large Cap Fund</t>
+  </si>
+  <si>
+    <t>HDFC Large Cap</t>
+  </si>
+  <si>
+    <t>HDFC Mid Cap Opportunities Fund</t>
+  </si>
+  <si>
+    <t>HDFC Multi Cap Fund</t>
+  </si>
+  <si>
+    <t>HDFC Small Cap Fund</t>
+  </si>
+  <si>
+    <t>ICICI Focused Equity</t>
+  </si>
+  <si>
+    <t>ICICI Prudential Bluechip Fund</t>
+  </si>
+  <si>
+    <t>ICICI Prudential Flexi Cap Fund</t>
+  </si>
+  <si>
+    <t>ICICI Prudential Focused Equity Fund</t>
+  </si>
+  <si>
+    <t>ICICI Prudential India Opportunities Fund</t>
+  </si>
+  <si>
+    <t>ICICI Prudential Large &amp; Mid Cap Fund</t>
+  </si>
+  <si>
+    <t>ICICI Prudential Mid Cap Fund</t>
+  </si>
+  <si>
+    <t>ICICI Prudential Multi Cap Fund</t>
+  </si>
+  <si>
+    <t>ICICI Prudential Value Discovery Fund</t>
+  </si>
+  <si>
+    <t>Kotak Blue Chip Fund</t>
+  </si>
+  <si>
+    <t>Kotak ESG Exclusionary Fund</t>
+  </si>
+  <si>
+    <t>Kotak Flexi Cap Fund</t>
+  </si>
+  <si>
+    <t>Kotak Large Cap Fund</t>
+  </si>
+  <si>
+    <t>Kotak Multi Cap Fund</t>
+  </si>
+  <si>
     <t>Kotak Multicap</t>
   </si>
   <si>
     <t xml:space="preserve">B </t>
   </si>
   <si>
-    <t>Axis ESG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A </t>
-  </si>
-  <si>
-    <t>Aditya Birla Nifty 50 Index</t>
-  </si>
-  <si>
-    <t>A</t>
+    <t>Kotak Pioneer Fund</t>
+  </si>
+  <si>
+    <t>Mirae Asset Large Cap Fund</t>
+  </si>
+  <si>
+    <t>Mirae Asset Midcap Fund</t>
+  </si>
+  <si>
+    <t>SBI Blue Chip Fund</t>
+  </si>
+  <si>
+    <t>SBI Contra Fund</t>
+  </si>
+  <si>
+    <t>SBI ESG Exclusionary Strategy Fund</t>
+  </si>
+  <si>
+    <t>SBI Flexi Cap Fund</t>
+  </si>
+  <si>
+    <t>SBI Focused Equity Fund</t>
+  </si>
+  <si>
+    <t>SBI Large &amp; Mid Cap Fund</t>
+  </si>
+  <si>
+    <t>SBI Multi Cap Fund</t>
+  </si>
+  <si>
+    <t>UTI Flexi Cap Fund</t>
+  </si>
+  <si>
+    <t>UTI Focused Fund</t>
+  </si>
+  <si>
+    <t>UTI Innovation Fund</t>
+  </si>
+  <si>
+    <t>UTI Large and Midcap Fund</t>
+  </si>
+  <si>
+    <t>UTI Large Cap Fund</t>
   </si>
   <si>
     <t>UTI Large Cap</t>
-  </si>
-  <si>
-    <t>ICICI Focused Equity</t>
-  </si>
-  <si>
-    <t>B+</t>
-  </si>
-  <si>
-    <t>HDFC Large Cap</t>
-  </si>
-  <si>
-    <t>HDFC Multi Cap Fund</t>
-  </si>
-  <si>
-    <t>HDFC Mid Cap Opportunities Fund</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>HDFC Large Cap Fund</t>
-  </si>
-  <si>
-    <t>HDFC Large Cap and Mid Cap Fund</t>
-  </si>
-  <si>
-    <t>HDFC Flexi Cap Fund</t>
-  </si>
-  <si>
-    <t>SBI Large &amp; Mid Cap Fund</t>
-  </si>
-  <si>
-    <t>SBI Blue Chip Fund</t>
-  </si>
-  <si>
-    <t>SBI Focused Equity Fund</t>
-  </si>
-  <si>
-    <t>SBI Flexi Cap Fund</t>
-  </si>
-  <si>
-    <t>SBI Multi Cap Fund</t>
-  </si>
-  <si>
-    <t>SBI ESG Exclusionary Strategy Fund</t>
-  </si>
-  <si>
-    <t>SBI Contra Fund</t>
-  </si>
-  <si>
-    <t>ICICI Prudential Bluechip Fund</t>
-  </si>
-  <si>
-    <t>ICICI Prudential Flexi Cap Fund</t>
-  </si>
-  <si>
-    <t>ICICI Prudential Focused Equity Fund</t>
-  </si>
-  <si>
-    <t>ICICI Prudential India Opportunities Fund</t>
-  </si>
-  <si>
-    <t>ICICI Prudential Large &amp; Mid Cap Fund</t>
-  </si>
-  <si>
-    <t>ICICI Prudential Mid Cap Fund</t>
-  </si>
-  <si>
-    <t>ICICI Prudential Multi Cap Fund</t>
-  </si>
-  <si>
-    <t>ICICI Prudential Value Discovery Fund</t>
-  </si>
-  <si>
-    <t>Kotak Flexi Cap Fund</t>
-  </si>
-  <si>
-    <t>Kotak Multi Cap Fund</t>
-  </si>
-  <si>
-    <t>Kotak Large Cap Fund</t>
-  </si>
-  <si>
-    <t>Kotak ESG Exclusionary Fund</t>
-  </si>
-  <si>
-    <t>Kotak Pioneer Fund</t>
-  </si>
-  <si>
-    <t>Kotak Blue Chip Fund</t>
-  </si>
-  <si>
-    <t>UTI Large and Midcap Fund</t>
-  </si>
-  <si>
-    <t>UTI Large Cap Fund</t>
-  </si>
-  <si>
-    <t>UTI Innovation Fund</t>
-  </si>
-  <si>
-    <t>UTI Flexi Cap Fund</t>
-  </si>
-  <si>
-    <t>UTI Focused Fund</t>
-  </si>
-  <si>
-    <t>Axis Multi Cap Fund</t>
-  </si>
-  <si>
-    <t>Axis Flexi Cap Fund</t>
-  </si>
-  <si>
-    <t>Axis Blue Chip Fund</t>
-  </si>
-  <si>
-    <t>Axis ESG Integration Strategy Fund</t>
-  </si>
-  <si>
-    <t>Axis Focused Fund</t>
-  </si>
-  <si>
-    <t>Axis Growth Opportunities Fund</t>
-  </si>
-  <si>
-    <t>Mirae Asset Large Cap Fund</t>
-  </si>
-  <si>
-    <t>Mirae Asset Midcap Fund</t>
-  </si>
-  <si>
-    <t>DSP Quant Fund</t>
-  </si>
-  <si>
-    <t>DSP Value Fund</t>
-  </si>
-  <si>
-    <t>DSP Nifty Next 50 Index Fund</t>
-  </si>
-  <si>
-    <t>DSP Flexi Cap Fund</t>
-  </si>
-  <si>
-    <t>HDFC Small Cap Fund</t>
-  </si>
-  <si>
-    <t>NR</t>
-  </si>
-  <si>
-    <t>DSP Multi Cap Fund</t>
   </si>
   <si>
     <t>Sr No.</t>
@@ -5450,7 +5450,7 @@
   </sheetPr>
   <dimension ref="A1:R501"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5583,7 +5583,7 @@
         <v>66</v>
       </c>
       <c r="R2" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
@@ -5639,7 +5639,7 @@
         <v>64</v>
       </c>
       <c r="R3" s="15" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -5695,7 +5695,7 @@
         <v>63</v>
       </c>
       <c r="R4" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -5751,7 +5751,7 @@
         <v>67</v>
       </c>
       <c r="R5" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
@@ -5807,7 +5807,7 @@
         <v>65</v>
       </c>
       <c r="R6" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
@@ -5863,7 +5863,7 @@
         <v>63</v>
       </c>
       <c r="R7" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
@@ -6087,7 +6087,7 @@
         <v>65</v>
       </c>
       <c r="R11" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
@@ -6143,7 +6143,7 @@
         <v>68</v>
       </c>
       <c r="R12" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
@@ -6255,7 +6255,7 @@
         <v>64</v>
       </c>
       <c r="R14" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
@@ -6367,7 +6367,7 @@
         <v>67</v>
       </c>
       <c r="R16" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
@@ -6423,7 +6423,7 @@
         <v>62</v>
       </c>
       <c r="R17" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
@@ -6479,7 +6479,7 @@
         <v>66</v>
       </c>
       <c r="R18" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
@@ -6535,7 +6535,7 @@
         <v>65</v>
       </c>
       <c r="R19" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
@@ -6815,7 +6815,7 @@
         <v>61</v>
       </c>
       <c r="R24" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
@@ -6927,7 +6927,7 @@
         <v>72</v>
       </c>
       <c r="R26" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
@@ -7039,7 +7039,7 @@
         <v>62</v>
       </c>
       <c r="R28" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
@@ -7151,7 +7151,7 @@
         <v>61</v>
       </c>
       <c r="R30" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
@@ -7207,7 +7207,7 @@
         <v>65</v>
       </c>
       <c r="R31" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
@@ -7319,7 +7319,7 @@
         <v>66</v>
       </c>
       <c r="R33" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
@@ -7599,7 +7599,7 @@
         <v>64</v>
       </c>
       <c r="R38" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
@@ -7655,7 +7655,7 @@
         <v>70</v>
       </c>
       <c r="R39" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
@@ -7711,7 +7711,7 @@
         <v>67</v>
       </c>
       <c r="R40" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
@@ -7767,7 +7767,7 @@
         <v>66</v>
       </c>
       <c r="R41" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
@@ -7991,7 +7991,7 @@
         <v>68</v>
       </c>
       <c r="R45" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
@@ -8047,7 +8047,7 @@
         <v>65</v>
       </c>
       <c r="R46" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
@@ -8103,7 +8103,7 @@
         <v>64</v>
       </c>
       <c r="R47" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
@@ -8215,7 +8215,7 @@
         <v>72</v>
       </c>
       <c r="R49" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
@@ -8439,7 +8439,7 @@
         <v>62</v>
       </c>
       <c r="R53" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
@@ -8495,7 +8495,7 @@
         <v>71</v>
       </c>
       <c r="R54" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
@@ -8719,7 +8719,7 @@
         <v>72</v>
       </c>
       <c r="R58" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
@@ -9111,7 +9111,7 @@
         <v>67</v>
       </c>
       <c r="R65" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
@@ -9167,7 +9167,7 @@
         <v>66</v>
       </c>
       <c r="R66" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
@@ -9447,7 +9447,7 @@
         <v>65</v>
       </c>
       <c r="R71" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
@@ -9503,7 +9503,7 @@
         <v>64</v>
       </c>
       <c r="R72" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
@@ -9559,7 +9559,7 @@
         <v>60</v>
       </c>
       <c r="R73" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
@@ -9951,7 +9951,7 @@
         <v>63</v>
       </c>
       <c r="R80" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
@@ -10119,7 +10119,7 @@
         <v>68</v>
       </c>
       <c r="R83" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
@@ -10175,7 +10175,7 @@
         <v>69</v>
       </c>
       <c r="R84" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
@@ -10565,7 +10565,7 @@
         <v>64</v>
       </c>
       <c r="R91" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
@@ -10677,7 +10677,7 @@
         <v>61</v>
       </c>
       <c r="R93" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
@@ -10733,7 +10733,7 @@
         <v>62</v>
       </c>
       <c r="R94" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
@@ -10899,7 +10899,7 @@
         <v>62</v>
       </c>
       <c r="R97" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
@@ -11011,7 +11011,7 @@
         <v>62</v>
       </c>
       <c r="R99" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
@@ -11179,7 +11179,7 @@
         <v>67</v>
       </c>
       <c r="R102" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
@@ -11403,7 +11403,7 @@
         <v>60</v>
       </c>
       <c r="R106" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
@@ -11459,7 +11459,7 @@
         <v>63</v>
       </c>
       <c r="R107" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
@@ -11795,7 +11795,7 @@
         <v>63</v>
       </c>
       <c r="R113" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
@@ -12187,7 +12187,7 @@
         <v>65</v>
       </c>
       <c r="R120" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
@@ -12243,7 +12243,7 @@
         <v>73</v>
       </c>
       <c r="R121" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
@@ -12299,7 +12299,7 @@
         <v>72</v>
       </c>
       <c r="R122" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
@@ -12355,7 +12355,7 @@
         <v>63</v>
       </c>
       <c r="R123" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
@@ -12411,7 +12411,7 @@
         <v>61</v>
       </c>
       <c r="R124" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
@@ -12523,7 +12523,7 @@
         <v>67</v>
       </c>
       <c r="R126" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
@@ -12747,7 +12747,7 @@
         <v>66</v>
       </c>
       <c r="R130" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
@@ -12915,7 +12915,7 @@
         <v>67</v>
       </c>
       <c r="R133" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
@@ -13027,7 +13027,7 @@
         <v>60</v>
       </c>
       <c r="R135" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
@@ -13139,7 +13139,7 @@
         <v>65</v>
       </c>
       <c r="R137" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
@@ -13307,7 +13307,7 @@
         <v>69</v>
       </c>
       <c r="R140" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
@@ -13419,7 +13419,7 @@
         <v>61</v>
       </c>
       <c r="R142" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
@@ -13475,7 +13475,7 @@
         <v>62</v>
       </c>
       <c r="R143" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
@@ -13923,7 +13923,7 @@
         <v>61</v>
       </c>
       <c r="R151" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
@@ -13979,7 +13979,7 @@
         <v>72</v>
       </c>
       <c r="R152" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
@@ -14203,7 +14203,7 @@
         <v>62</v>
       </c>
       <c r="R156" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
@@ -14259,7 +14259,7 @@
         <v>74</v>
       </c>
       <c r="R157" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
@@ -14483,7 +14483,7 @@
         <v>68</v>
       </c>
       <c r="R161" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
@@ -14707,7 +14707,7 @@
         <v>64</v>
       </c>
       <c r="R165" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
@@ -14819,7 +14819,7 @@
         <v>63</v>
       </c>
       <c r="R167" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
@@ -14931,7 +14931,7 @@
         <v>65</v>
       </c>
       <c r="R169" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
@@ -14987,7 +14987,7 @@
         <v>72</v>
       </c>
       <c r="R170" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
@@ -15043,7 +15043,7 @@
         <v>63</v>
       </c>
       <c r="R171" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
@@ -15099,7 +15099,7 @@
         <v>64</v>
       </c>
       <c r="R172" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
@@ -15379,7 +15379,7 @@
         <v>69</v>
       </c>
       <c r="R177" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
@@ -15435,7 +15435,7 @@
         <v>67</v>
       </c>
       <c r="R178" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
@@ -15491,7 +15491,7 @@
         <v>63</v>
       </c>
       <c r="R179" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
@@ -16107,7 +16107,7 @@
         <v>61</v>
       </c>
       <c r="R190" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="191" customHeight="1" ht="18.75">
@@ -16219,7 +16219,7 @@
         <v>64</v>
       </c>
       <c r="R192" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="18.75">
@@ -16387,7 +16387,7 @@
         <v>72</v>
       </c>
       <c r="R195" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="18.75">
@@ -16499,7 +16499,7 @@
         <v>73</v>
       </c>
       <c r="R197" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="198" customHeight="1" ht="18.75">
@@ -16555,7 +16555,7 @@
         <v>73</v>
       </c>
       <c r="R198" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="199" customHeight="1" ht="18.75">
@@ -16611,7 +16611,7 @@
         <v>66</v>
       </c>
       <c r="R199" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="200" customHeight="1" ht="18.75">
@@ -16667,7 +16667,7 @@
         <v>68</v>
       </c>
       <c r="R200" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="201" customHeight="1" ht="18.75">
@@ -16723,7 +16723,7 @@
         <v>62</v>
       </c>
       <c r="R201" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="202" customHeight="1" ht="18.75">
@@ -17003,7 +17003,7 @@
         <v>68</v>
       </c>
       <c r="R206" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="18.75">
@@ -17059,7 +17059,7 @@
         <v>61</v>
       </c>
       <c r="R207" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="18.75">
@@ -17171,7 +17171,7 @@
         <v>68</v>
       </c>
       <c r="R209" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="18.75">
@@ -17451,7 +17451,7 @@
         <v>61</v>
       </c>
       <c r="R214" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="18.75">
@@ -17507,7 +17507,7 @@
         <v>65</v>
       </c>
       <c r="R215" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="216" customHeight="1" ht="18.75">
@@ -17563,7 +17563,7 @@
         <v>63</v>
       </c>
       <c r="R216" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="217" customHeight="1" ht="18.75">
@@ -17843,7 +17843,7 @@
         <v>66</v>
       </c>
       <c r="R221" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="18.75">
@@ -18235,7 +18235,7 @@
         <v>68</v>
       </c>
       <c r="R228" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="18.75">
@@ -18291,7 +18291,7 @@
         <v>68</v>
       </c>
       <c r="R229" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="18.75">
@@ -18403,7 +18403,7 @@
         <v>67</v>
       </c>
       <c r="R231" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="18.75">
@@ -18515,7 +18515,7 @@
         <v>67</v>
       </c>
       <c r="R233" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="18.75">
@@ -18627,7 +18627,7 @@
         <v>62</v>
       </c>
       <c r="R235" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="236" customHeight="1" ht="18.75">
@@ -18739,7 +18739,7 @@
         <v>61</v>
       </c>
       <c r="R237" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="238" customHeight="1" ht="18.75">
@@ -18851,7 +18851,7 @@
         <v>62</v>
       </c>
       <c r="R239" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="240" customHeight="1" ht="18.75">
@@ -19467,7 +19467,7 @@
         <v>63</v>
       </c>
       <c r="R250" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="251" customHeight="1" ht="18.75">
@@ -19579,7 +19579,7 @@
         <v>62</v>
       </c>
       <c r="R252" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="253" customHeight="1" ht="18.75">
@@ -19635,7 +19635,7 @@
         <v>67</v>
       </c>
       <c r="R253" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="254" customHeight="1" ht="18.75">
@@ -19747,7 +19747,7 @@
         <v>73</v>
       </c>
       <c r="R255" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="256" customHeight="1" ht="18.75">
@@ -20083,7 +20083,7 @@
         <v>74</v>
       </c>
       <c r="R261" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="262" customHeight="1" ht="18.75">
@@ -20307,7 +20307,7 @@
         <v>61</v>
       </c>
       <c r="R265" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="266" customHeight="1" ht="18.75">
@@ -20475,7 +20475,7 @@
         <v>66</v>
       </c>
       <c r="R268" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="269" customHeight="1" ht="18.75">
@@ -20587,7 +20587,7 @@
         <v>68</v>
       </c>
       <c r="R270" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="271" customHeight="1" ht="18.75">
@@ -20699,7 +20699,7 @@
         <v>61</v>
       </c>
       <c r="R272" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="273" customHeight="1" ht="18.75">
@@ -20811,7 +20811,7 @@
         <v>68</v>
       </c>
       <c r="R274" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="275" customHeight="1" ht="18.75">
@@ -20867,7 +20867,7 @@
         <v>69</v>
       </c>
       <c r="R275" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="276" customHeight="1" ht="18.75">
@@ -20923,7 +20923,7 @@
         <v>68</v>
       </c>
       <c r="R276" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="277" customHeight="1" ht="18.75">
@@ -21035,7 +21035,7 @@
         <v>67</v>
       </c>
       <c r="R278" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="279" customHeight="1" ht="18.75">
@@ -21203,7 +21203,7 @@
         <v>72</v>
       </c>
       <c r="R281" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="282" customHeight="1" ht="18.75">
@@ -21259,7 +21259,7 @@
         <v>73</v>
       </c>
       <c r="R282" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="283" customHeight="1" ht="18.75">
@@ -21315,7 +21315,7 @@
         <v>64</v>
       </c>
       <c r="R283" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="284" customHeight="1" ht="18.75">
@@ -21371,7 +21371,7 @@
         <v>65</v>
       </c>
       <c r="R284" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="285" customHeight="1" ht="18.75">
@@ -21483,7 +21483,7 @@
         <v>69</v>
       </c>
       <c r="R286" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="287" customHeight="1" ht="18.75">
@@ -21651,7 +21651,7 @@
         <v>61</v>
       </c>
       <c r="R289" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="290" customHeight="1" ht="18.75">
@@ -21875,7 +21875,7 @@
         <v>66</v>
       </c>
       <c r="R293" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="294" customHeight="1" ht="18.75">
@@ -21931,7 +21931,7 @@
         <v>74</v>
       </c>
       <c r="R294" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="295" customHeight="1" ht="18.75">
@@ -22211,7 +22211,7 @@
         <v>67</v>
       </c>
       <c r="R299" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="300" customHeight="1" ht="18.75">
@@ -22379,7 +22379,7 @@
         <v>69</v>
       </c>
       <c r="R302" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="303" customHeight="1" ht="18.75">
@@ -22491,7 +22491,7 @@
         <v>70</v>
       </c>
       <c r="R304" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="305" customHeight="1" ht="18.75">
@@ -22547,7 +22547,7 @@
         <v>64</v>
       </c>
       <c r="R305" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="306" customHeight="1" ht="18.75">
@@ -22603,7 +22603,7 @@
         <v>68</v>
       </c>
       <c r="R306" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="307" customHeight="1" ht="18.75">
@@ -22827,7 +22827,7 @@
         <v>63</v>
       </c>
       <c r="R310" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="311" customHeight="1" ht="18.75">
@@ -22995,7 +22995,7 @@
         <v>71</v>
       </c>
       <c r="R313" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="314" customHeight="1" ht="18.75">
@@ -23275,7 +23275,7 @@
         <v>68</v>
       </c>
       <c r="R318" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="319" customHeight="1" ht="18.75">
@@ -23331,7 +23331,7 @@
         <v>69</v>
       </c>
       <c r="R319" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="320" customHeight="1" ht="18.75">
@@ -23611,7 +23611,7 @@
         <v>65</v>
       </c>
       <c r="R324" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="325" customHeight="1" ht="18.75">
@@ -23667,7 +23667,7 @@
         <v>63</v>
       </c>
       <c r="R325" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="326" customHeight="1" ht="18.75">
@@ -23779,7 +23779,7 @@
         <v>68</v>
       </c>
       <c r="R327" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="328" customHeight="1" ht="18.75">
@@ -23891,7 +23891,7 @@
         <v>64</v>
       </c>
       <c r="R329" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="330" customHeight="1" ht="18.75">
@@ -24115,7 +24115,7 @@
         <v>63</v>
       </c>
       <c r="R333" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="334" customHeight="1" ht="18.75">
@@ -24283,7 +24283,7 @@
         <v>64</v>
       </c>
       <c r="R336" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="337" customHeight="1" ht="18.75">
@@ -24507,7 +24507,7 @@
         <v>62</v>
       </c>
       <c r="R340" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="341" customHeight="1" ht="18.75">
@@ -24619,7 +24619,7 @@
         <v>61</v>
       </c>
       <c r="R342" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="343" customHeight="1" ht="18.75">
@@ -24787,7 +24787,7 @@
         <v>69</v>
       </c>
       <c r="R345" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="346" customHeight="1" ht="18.75">
@@ -24955,7 +24955,7 @@
         <v>64</v>
       </c>
       <c r="R348" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="349" customHeight="1" ht="18.75">
@@ -25011,7 +25011,7 @@
         <v>62</v>
       </c>
       <c r="R349" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="350" customHeight="1" ht="18.75">
@@ -25067,7 +25067,7 @@
         <v>70</v>
       </c>
       <c r="R350" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="351" customHeight="1" ht="18.75">
@@ -25123,7 +25123,7 @@
         <v>66</v>
       </c>
       <c r="R351" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="352" customHeight="1" ht="18.75">
@@ -25179,7 +25179,7 @@
         <v>63</v>
       </c>
       <c r="R352" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="353" customHeight="1" ht="18.75">
@@ -25235,7 +25235,7 @@
         <v>61</v>
       </c>
       <c r="R353" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="354" customHeight="1" ht="18.75">
@@ -25403,7 +25403,7 @@
         <v>62</v>
       </c>
       <c r="R356" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="357" customHeight="1" ht="18.75">
@@ -25571,7 +25571,7 @@
         <v>68</v>
       </c>
       <c r="R359" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="360" customHeight="1" ht="18.75">
@@ -25627,7 +25627,7 @@
         <v>63</v>
       </c>
       <c r="R360" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="361" customHeight="1" ht="18.75">
@@ -25683,7 +25683,7 @@
         <v>62</v>
       </c>
       <c r="R361" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="362" customHeight="1" ht="18.75">
@@ -25739,7 +25739,7 @@
         <v>61</v>
       </c>
       <c r="R362" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="363" customHeight="1" ht="18.75">
@@ -25851,7 +25851,7 @@
         <v>62</v>
       </c>
       <c r="R364" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="365" customHeight="1" ht="18.75">
@@ -26075,7 +26075,7 @@
         <v>65</v>
       </c>
       <c r="R368" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="369" customHeight="1" ht="18.75">
@@ -26299,7 +26299,7 @@
         <v>71</v>
       </c>
       <c r="R372" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="373" customHeight="1" ht="18.75">
@@ -26411,7 +26411,7 @@
         <v>63</v>
       </c>
       <c r="R374" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="375" customHeight="1" ht="18.75">
@@ -26691,7 +26691,7 @@
         <v>65</v>
       </c>
       <c r="R379" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="380" customHeight="1" ht="18.75">
@@ -26859,7 +26859,7 @@
         <v>62</v>
       </c>
       <c r="R382" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="383" customHeight="1" ht="18.75">
@@ -26915,7 +26915,7 @@
         <v>60</v>
       </c>
       <c r="R383" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="384" customHeight="1" ht="18.75">
@@ -27195,7 +27195,7 @@
         <v>64</v>
       </c>
       <c r="R388" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="389" customHeight="1" ht="18.75">
@@ -27307,7 +27307,7 @@
         <v>66</v>
       </c>
       <c r="R390" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="391" customHeight="1" ht="18.75">
@@ -27363,7 +27363,7 @@
         <v>70</v>
       </c>
       <c r="R391" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="392" customHeight="1" ht="18.75">
@@ -27419,7 +27419,7 @@
         <v>72</v>
       </c>
       <c r="R392" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="393" customHeight="1" ht="18.75">
@@ -27699,7 +27699,7 @@
         <v>66</v>
       </c>
       <c r="R397" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="398" customHeight="1" ht="18.75">
@@ -27755,7 +27755,7 @@
         <v>68</v>
       </c>
       <c r="R398" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="399" customHeight="1" ht="18.75">
@@ -27811,7 +27811,7 @@
         <v>62</v>
       </c>
       <c r="R399" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="400" customHeight="1" ht="18.75">
@@ -28091,7 +28091,7 @@
         <v>61</v>
       </c>
       <c r="R404" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="405" customHeight="1" ht="18.75">
@@ -28257,7 +28257,7 @@
         <v>71</v>
       </c>
       <c r="R407" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="408" customHeight="1" ht="18.75">
@@ -28369,7 +28369,7 @@
         <v>61</v>
       </c>
       <c r="R409" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="410" customHeight="1" ht="18.75">
@@ -28425,7 +28425,7 @@
         <v>67</v>
       </c>
       <c r="R410" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="411" customHeight="1" ht="18.75">
@@ -28537,7 +28537,7 @@
         <v>64</v>
       </c>
       <c r="R412" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="413" customHeight="1" ht="18.75">
@@ -28593,7 +28593,7 @@
         <v>62</v>
       </c>
       <c r="R413" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="414" customHeight="1" ht="18.75">
@@ -29153,7 +29153,7 @@
         <v>70</v>
       </c>
       <c r="R423" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="424" customHeight="1" ht="18.75">
@@ -29377,7 +29377,7 @@
         <v>62</v>
       </c>
       <c r="R427" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="428" customHeight="1" ht="18.75">
@@ -29489,7 +29489,7 @@
         <v>66</v>
       </c>
       <c r="R429" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="430" customHeight="1" ht="18.75">
@@ -29545,7 +29545,7 @@
         <v>66</v>
       </c>
       <c r="R430" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="431" customHeight="1" ht="18.75">
@@ -29657,7 +29657,7 @@
         <v>74</v>
       </c>
       <c r="R432" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="433" customHeight="1" ht="18.75">
@@ -29713,7 +29713,7 @@
         <v>64</v>
       </c>
       <c r="R433" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="434" customHeight="1" ht="18.75">
@@ -29769,7 +29769,7 @@
         <v>72</v>
       </c>
       <c r="R434" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="435" customHeight="1" ht="18.75">
@@ -29937,7 +29937,7 @@
         <v>71</v>
       </c>
       <c r="R437" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="438" customHeight="1" ht="18.75">
@@ -29993,7 +29993,7 @@
         <v>73</v>
       </c>
       <c r="R438" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="439" customHeight="1" ht="18.75">
@@ -30049,7 +30049,7 @@
         <v>73</v>
       </c>
       <c r="R439" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="440" customHeight="1" ht="18.75">
@@ -30217,7 +30217,7 @@
         <v>67</v>
       </c>
       <c r="R442" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="443" customHeight="1" ht="18.75">
@@ -30329,7 +30329,7 @@
         <v>69</v>
       </c>
       <c r="R444" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="445" customHeight="1" ht="18.75">
@@ -30385,7 +30385,7 @@
         <v>62</v>
       </c>
       <c r="R445" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="446" customHeight="1" ht="18.75">
@@ -30665,7 +30665,7 @@
         <v>73</v>
       </c>
       <c r="R450" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="451" customHeight="1" ht="18.75">
@@ -30721,7 +30721,7 @@
         <v>69</v>
       </c>
       <c r="R451" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="452" customHeight="1" ht="18.75">
@@ -30777,7 +30777,7 @@
         <v>69</v>
       </c>
       <c r="R452" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="453" customHeight="1" ht="18.75">
@@ -31057,7 +31057,7 @@
         <v>70</v>
       </c>
       <c r="R457" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="458" customHeight="1" ht="18.75">
@@ -31225,7 +31225,7 @@
         <v>65</v>
       </c>
       <c r="R460" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="461" customHeight="1" ht="18.75">
@@ -31281,7 +31281,7 @@
         <v>60</v>
       </c>
       <c r="R461" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="462" customHeight="1" ht="18.75">
@@ -31337,7 +31337,7 @@
         <v>65</v>
       </c>
       <c r="R462" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="463" customHeight="1" ht="18.75">
@@ -31393,7 +31393,7 @@
         <v>74</v>
       </c>
       <c r="R463" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="464" customHeight="1" ht="18.75">
@@ -31449,7 +31449,7 @@
         <v>68</v>
       </c>
       <c r="R464" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="465" customHeight="1" ht="18.75">
@@ -31729,7 +31729,7 @@
         <v>67</v>
       </c>
       <c r="R469" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="470" customHeight="1" ht="18.75">
@@ -31897,7 +31897,7 @@
         <v>63</v>
       </c>
       <c r="R472" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="473" customHeight="1" ht="18.75">
@@ -31953,7 +31953,7 @@
         <v>68</v>
       </c>
       <c r="R473" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="474" customHeight="1" ht="18.75">
@@ -32121,7 +32121,7 @@
         <v>75</v>
       </c>
       <c r="R476" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="477" customHeight="1" ht="18.75">
@@ -32177,7 +32177,7 @@
         <v>65</v>
       </c>
       <c r="R477" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="478" customHeight="1" ht="18.75">
@@ -32289,7 +32289,7 @@
         <v>72</v>
       </c>
       <c r="R479" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="480" customHeight="1" ht="18.75">
@@ -32401,7 +32401,7 @@
         <v>67</v>
       </c>
       <c r="R481" s="15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="482" customHeight="1" ht="18.75">
@@ -32457,7 +32457,7 @@
         <v>62</v>
       </c>
       <c r="R482" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="483" customHeight="1" ht="18.75">
@@ -32737,7 +32737,7 @@
         <v>65</v>
       </c>
       <c r="R487" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="488" customHeight="1" ht="18.75">
@@ -33017,7 +33017,7 @@
         <v>63</v>
       </c>
       <c r="R492" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="493" customHeight="1" ht="18.75">
@@ -33185,7 +33185,7 @@
         <v>72</v>
       </c>
       <c r="R495" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="496" customHeight="1" ht="18.75">
@@ -33241,7 +33241,7 @@
         <v>71</v>
       </c>
       <c r="R496" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="497" customHeight="1" ht="18.75">
@@ -33297,7 +33297,7 @@
         <v>73</v>
       </c>
       <c r="R497" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="498" customHeight="1" ht="18.75">
@@ -33353,7 +33353,7 @@
         <v>74</v>
       </c>
       <c r="R498" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="499" customHeight="1" ht="18.75">
@@ -33465,7 +33465,7 @@
         <v>72</v>
       </c>
       <c r="R500" s="15" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="501" customHeight="1" ht="18.75">
@@ -33536,7 +33536,7 @@
   </sheetPr>
   <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -33550,103 +33550,103 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="2">
+        <v>70</v>
+      </c>
+      <c r="C1" s="3">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" s="4">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C3" s="5">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" s="4">
         <v>70</v>
       </c>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C5" s="5">
-        <v>0.99</v>
+        <v>0.97</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="5">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B7" s="4">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C7" s="5">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4">
         <v>65</v>
@@ -33655,91 +33655,91 @@
         <v>0.9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B9" s="4">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C9" s="5">
-        <v>0.94</v>
+        <v>0.97</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B10" s="4">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C10" s="5">
-        <v>0.99</v>
+        <v>0.84</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C11" s="5">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B12" s="4">
         <v>70</v>
       </c>
       <c r="C12" s="5">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B13" s="4">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C13" s="5">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="B14" s="4">
-        <v>69</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
@@ -33747,13 +33747,13 @@
         <v>22</v>
       </c>
       <c r="B15" s="4">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C15" s="5">
-        <v>0.91</v>
+        <v>0.97</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
@@ -33761,13 +33761,13 @@
         <v>23</v>
       </c>
       <c r="B16" s="4">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C16" s="5">
         <v>0.97</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
@@ -33775,13 +33775,13 @@
         <v>24</v>
       </c>
       <c r="B17" s="4">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="C17" s="5">
-        <v>0.88</v>
+        <v>0.99</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
@@ -33789,13 +33789,13 @@
         <v>25</v>
       </c>
       <c r="B18" s="4">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C18" s="5">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
@@ -33803,13 +33803,13 @@
         <v>26</v>
       </c>
       <c r="B19" s="4">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C19" s="5">
-        <v>0.96</v>
+        <v>0.94</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
@@ -33817,13 +33817,13 @@
         <v>27</v>
       </c>
       <c r="B20" s="4">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C20" s="5">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
@@ -33831,13 +33831,13 @@
         <v>28</v>
       </c>
       <c r="B21" s="4">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C21" s="5">
-        <v>0.86</v>
+        <v>0.64</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
@@ -33848,10 +33848,10 @@
         <v>68</v>
       </c>
       <c r="C22" s="5">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
@@ -33859,13 +33859,13 @@
         <v>30</v>
       </c>
       <c r="B23" s="4">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C23" s="5">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
@@ -33873,13 +33873,13 @@
         <v>31</v>
       </c>
       <c r="B24" s="4">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C24" s="5">
-        <v>0.99</v>
+        <v>0.86</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
@@ -33887,13 +33887,13 @@
         <v>32</v>
       </c>
       <c r="B25" s="4">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="C25" s="5">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
@@ -33901,13 +33901,13 @@
         <v>33</v>
       </c>
       <c r="B26" s="4">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C26" s="5">
-        <v>0.93</v>
+        <v>0.98</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
@@ -33915,13 +33915,13 @@
         <v>34</v>
       </c>
       <c r="B27" s="4">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C27" s="5">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
@@ -33929,13 +33929,13 @@
         <v>35</v>
       </c>
       <c r="B28" s="4">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C28" s="5">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
@@ -33943,13 +33943,13 @@
         <v>36</v>
       </c>
       <c r="B29" s="4">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C29" s="5">
-        <v>0.87</v>
+        <v>0.93</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
@@ -33957,13 +33957,13 @@
         <v>37</v>
       </c>
       <c r="B30" s="4">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C30" s="5">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
@@ -33971,13 +33971,13 @@
         <v>38</v>
       </c>
       <c r="B31" s="4">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" s="5">
         <v>0.98</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
@@ -33985,13 +33985,13 @@
         <v>39</v>
       </c>
       <c r="B32" s="4">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C32" s="5">
-        <v>0.89</v>
+        <v>0.98</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
@@ -33999,13 +33999,13 @@
         <v>40</v>
       </c>
       <c r="B33" s="4">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C33" s="5">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
@@ -34016,10 +34016,10 @@
         <v>65</v>
       </c>
       <c r="C34" s="5">
-        <v>0.93</v>
+        <v>0.99</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
@@ -34027,13 +34027,13 @@
         <v>42</v>
       </c>
       <c r="B35" s="4">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C35" s="5">
-        <v>0.99</v>
+        <v>0.87</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
@@ -34041,223 +34041,223 @@
         <v>43</v>
       </c>
       <c r="B36" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C36" s="5">
-        <v>0.89</v>
+        <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B37" s="4">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C37" s="5">
-        <v>0.99</v>
+        <v>0.89</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B38" s="4">
         <v>68</v>
       </c>
       <c r="C38" s="5">
-        <v>1</v>
+        <v>0.99</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B39" s="4">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C39" s="5">
-        <v>0.9</v>
+        <v>0.93</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B40" s="4">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C40" s="5">
-        <v>0.97</v>
+        <v>1</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B41" s="4">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C41" s="5">
-        <v>1</v>
+        <v>0.96</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B42" s="4">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C42" s="5">
-        <v>0.98</v>
+        <v>1</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
       <c r="A43" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B43" s="4">
         <v>67</v>
       </c>
       <c r="C43" s="5">
-        <v>1</v>
+        <v>0.97</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
       <c r="A44" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B44" s="4">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C44" s="5">
-        <v>0.95</v>
+        <v>0.91</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
       <c r="A45" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B45" s="4">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C45" s="5">
-        <v>0.99</v>
+        <v>0.95</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
       <c r="A46" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B46" s="4">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C46" s="5">
-        <v>0.93</v>
+        <v>0.88</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
       <c r="A47" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B47" s="4">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C47" s="5">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
       <c r="A48" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B48" s="4">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C48" s="5">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
       <c r="A49" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B49" s="4">
         <v>62</v>
       </c>
       <c r="C49" s="5">
-        <v>0.98</v>
+        <v>0.89</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
       <c r="A50" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B50" s="4">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" s="5">
-        <v>0.97</v>
+        <v>0.93</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
       <c r="A51" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B51" s="4">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C51" s="5">
-        <v>0.64</v>
+        <v>0.99</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
@@ -34265,13 +34265,13 @@
         <v>60</v>
       </c>
       <c r="B52" s="4">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C52" s="5">
-        <v>0.84</v>
+        <v>0.99</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>